<commit_message>
update excle& delete boss txt
Change-Id: I1c916370fba0c35ccc16873449907d9d66f5e23b
</commit_message>
<xml_diff>
--- a/data/FDD接口测试用例.xlsx
+++ b/data/FDD接口测试用例.xlsx
@@ -16,6 +16,7 @@
     <sheet name="saas_rent" r:id="rId10" sheetId="8"/>
     <sheet name="ddmf" r:id="rId11" sheetId="9"/>
     <sheet name="ddxfapp" r:id="rId12" sheetId="10"/>
+    <sheet name="ddjj" r:id="rId13" sheetId="11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="true">ddsf!$B$1:$B$301</definedName>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18661" uniqueCount="2132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19108" uniqueCount="2197">
   <si>
     <t>环境</t>
   </si>
@@ -9100,6 +9101,365 @@
   </si>
   <si>
     <t>客户手机号变更审核（第三次）</t>
+  </si>
+  <si>
+    <t>{'Content-Length': '55',
+'pragma': 'no-cache',
+                'Accept': '*/*',
+                'User-Agent': 'Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/78.0.3904.70 Safari/537.36',
+'elastic-apm-traceparent':'00-e71bde17e8160779e20797fd0f446f23-d74bda9818a699c2-01',
+                'Content-Type': 'application/json',
+'Origin': 'https://ddjj.fangdd.net',
+'Sec-Fetch-Site': 'same-origin',
+'Sec-Fetch-Mode': 'cors',
+'Referer': 'https://ddjj.fangdd.net/login',
+'x-requested-with': 'XMLHttpRequest',
+                'Accept-Encoding': 'gzip,deflate,br',
+                'Accept-Language': 'zh-CN,zh;q=0.9'
+            }</t>
+  </si>
+  <si>
+    <t>{"mode":1,"userName":"19900020002","password":"111111"}</t>
+  </si>
+  <si>
+    <t>{"code": "00000"}</t>
+  </si>
+  <si>
+    <t>aCommissionStatistic</t>
+  </si>
+  <si>
+    <t>结佣统计数据</t>
+  </si>
+  <si>
+    <t>{
+'pragma': 'no-cache',
+                'Accept': 'application/json, text/plain,*/*',
+                'User-Agent': 'Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/78.0.3904.70 Safari/537.36',
+'elastic-apm-traceparent':'00-e71bde17e8160779e20797fd0f446f23-d74bda9818a699c2-01',
+'Sec-Fetch-Site': 'same-origin',
+'Sec-Fetch-Mode': 'cors',
+'x-requested-with': 'XMLHttpRequest',
+                'Accept-Encoding': 'gzip,deflate,br',
+                'Accept-Language': 'zh-CN,zh;q=0.9',
+'User-Id':#userId#,
+'Token':#token#,
+'Cookie': #cookies#
+            }</t>
+  </si>
+  <si>
+    <t>bcommissionorg</t>
+  </si>
+  <si>
+    <t>结佣组织</t>
+  </si>
+  <si>
+    <t>{
+'pragma': 'no-cache',
+                'Accept': 'application/json, text/plain,*/*',
+                'User-Agent': 'Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/78.0.3904.70 Safari/537.36',
+'elastic-apm-traceparent':'00-e71bde17e8160779e20797fd0f446f23-d74bda9818a699c2-01',
+'Sec-Fetch-Site': 'same-origin',
+'Sec-Fetch-Mode': 'cors',
+'x-requested-with': 'XMLHttpRequest',
+                'Accept-Encoding': 'gzip,deflate,br',
+                'Accept-Language': 'zh-CN,zh;q=0.9',
+'Company-Id':'80159954',
+'User-Id':#userId#,
+'Token':#token#,
+'Cookie': #cookies#
+            }</t>
+  </si>
+  <si>
+    <t>cCommissionList</t>
+  </si>
+  <si>
+    <t>请佣单列表</t>
+  </si>
+  <si>
+    <t>{"relateType":"relateOut","relateData":[{"hash_commissionApplyId":"hash_commissionApplyId"},{"commissionApplyType":"commissionApplyType"}]}</t>
+  </si>
+  <si>
+    <t>{"pageNo":1,"pageSize":10,"commissionApplyStatus":0}</t>
+  </si>
+  <si>
+    <t>dCommissionFactoringInfo</t>
+  </si>
+  <si>
+    <t>{"commissionApplyType":#commissionApplyType#,"commissionApplyId":#hash_commissionApplyId#}</t>
+  </si>
+  <si>
+    <t>exfProtocolList</t>
+  </si>
+  <si>
+    <t>新房协议列表</t>
+  </si>
+  <si>
+    <t>fxfProtocolInfo</t>
+  </si>
+  <si>
+    <t>新房协议详情</t>
+  </si>
+  <si>
+    <t>{
+'pragma': 'no-cache',
+                'Accept': 'application/json, text/plain,*/*',
+                'User-Agent': 'Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/78.0.3904.70 Safari/537.36',
+'elastic-apm-traceparent':'00-e71bde17e8160779e20797fd0f446f23-d74bda9818a699c2-01',
+'Sec-Fetch-Site': 'same-origin',
+'Sec-Fetch-Mode': 'cors',
+'x-requested-with': 'XMLHttpRequest',
+                'Accept-Encoding': 'gzip,deflate,br',
+                'Accept-Language': 'zh-CN,zh;q=0.9',
+'Restful':'{"agreementSignId":30601}',
+'Company-Id':'80159954',
+'User-Id':#userId#,
+'Token':#token#,
+'Cookie': #cookies#
+            }</t>
+  </si>
+  <si>
+    <t>gReferralList</t>
+  </si>
+  <si>
+    <t>{"pageNo":1,"pageSize":20,"dateTypes":2,"contributorStoreIds":"80159961"}</t>
+  </si>
+  <si>
+    <t>{"code": 200}</t>
+  </si>
+  <si>
+    <t>hGuideList</t>
+  </si>
+  <si>
+    <t>iOrderList</t>
+  </si>
+  <si>
+    <t>成交列表</t>
+  </si>
+  <si>
+    <t>{"pageNo":1,"pageSize":20,"channelType":1,"dateTypes":2,"contributorStoreIds":"80159961"}</t>
+  </si>
+  <si>
+    <t>jAcountList</t>
+  </si>
+  <si>
+    <t>结佣主体列表</t>
+  </si>
+  <si>
+    <t>kOperator</t>
+  </si>
+  <si>
+    <t>操作人验证</t>
+  </si>
+  <si>
+    <t>{"enterpriseId":"66879"}</t>
+  </si>
+  <si>
+    <t>lProjectList</t>
+  </si>
+  <si>
+    <t>结佣项目列表</t>
+  </si>
+  <si>
+    <t>mApplyProtocolUrl</t>
+  </si>
+  <si>
+    <t>获取结佣协议</t>
+  </si>
+  <si>
+    <t>{"projectId":"14673"}</t>
+  </si>
+  <si>
+    <t>nSettlementList</t>
+  </si>
+  <si>
+    <t>结佣列表</t>
+  </si>
+  <si>
+    <t>{"relateType":"relateOut","relateData":[{"factoringCommissionId":"factoringCommissionId"}]}</t>
+  </si>
+  <si>
+    <t>{"projectId":"14673","enterpriseId":"66879"}</t>
+  </si>
+  <si>
+    <t>oBankAcountList</t>
+  </si>
+  <si>
+    <t>银行账户列表</t>
+  </si>
+  <si>
+    <t>{"enterpriseId":"66879","fundChannelCode":"JG"}</t>
+  </si>
+  <si>
+    <t>paddFastSettlement</t>
+  </si>
+  <si>
+    <t>{
+'pragma': 'no-cache',
+'Content-Type':'application/json;charset=UTF-8',
+                'Accept': 'application/json, text/plain,*/*',
+                'User-Agent': 'Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/78.0.3904.70 Safari/537.36',
+'elastic-apm-traceparent':'00-e71bde17e8160779e20797fd0f446f23-d74bda9818a699c2-01',
+'Sec-Fetch-Site': 'same-origin',
+'Sec-Fetch-Mode': 'cors',
+'x-requested-with': 'XMLHttpRequest',
+                'Accept-Encoding': 'gzip,deflate,br',
+                'Accept-Language': 'zh-CN,zh;q=0.9',
+'Company-Id':'80159954',
+'User-Id':#userId#,
+'Token':#token#,
+'Cookie': #cookies#
+            }</t>
+  </si>
+  <si>
+    <t>{"relateType":"relateOut","relateData":[{"hash_commissionApplyId":"hash_commissionApplyId"}]}</t>
+  </si>
+  <si>
+    <t>{"branchId":3,"factoringCommissionIds":[#factoringCommissionId#],"bankAccountId":50668,"enterpriseId":"66879"}</t>
+  </si>
+  <si>
+    <t>qFactoringCancel</t>
+  </si>
+  <si>
+    <t>{
+'pragma': 'no-cache',
+'Content-Type':'application/json;charset=UTF-8',
+                'Accept': 'application/json, text/plain,*/*',
+                'User-Agent': 'Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/78.0.3904.70 Safari/537.36',
+'elastic-apm-traceparent':'00-e71bde17e8160779e20797fd0f446f23-d74bda9818a699c2-01',
+'Sec-Fetch-Site': 'same-origin',
+'Sec-Fetch-Mode': 'cors',
+'x-requested-with': 'XMLHttpRequest',
+                'Accept-Encoding': 'gzip,deflate,br',
+                'Accept-Language': 'zh-CN,zh;q=0.9',
+'Company-Id':'80159954',
+'Restful':#hash_commissionApplyId#,
+'User-Id':#userId#,
+'Token':#token#,
+'Cookie': #cookies#
+            }</t>
+  </si>
+  <si>
+    <t>{'Content-Length': '55',
+'pragma': 'no-cache',
+                'Accept': '*/*',
+                'User-Agent': 'Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/78.0.3904.70 Safari/537.36',
+                'Content-Type': 'application/json',
+'Sec-Fetch-Site': 'same-origin',
+'Sec-Fetch-Mode': 'cors',
+'x-requested-with': 'XMLHttpRequest',
+                'Accept-Encoding': 'gzip,deflate,br',
+                'Accept-Language': 'zh-CN,zh;q=0.9'
+            }</t>
+  </si>
+  <si>
+    <t>{"mode":1,"userName":"13632596325","password":"123456"}</t>
+  </si>
+  <si>
+    <t>{
+'pragma': 'no-cache',
+                'Accept': 'application/json, text/plain,*/*',
+                'User-Agent': 'Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/78.0.3904.70 Safari/537.36',
+'Sec-Fetch-Site': 'same-origin',
+'Sec-Fetch-Mode': 'cors',
+'x-requested-with': 'XMLHttpRequest',
+                'Accept-Encoding': 'gzip,deflate,br',
+                'Accept-Language': 'zh-CN,zh;q=0.9',
+'User-Id':#userId#,
+'Token':#token#,
+'Cookie': #cookies#
+            }</t>
+  </si>
+  <si>
+    <t>{
+'pragma': 'no-cache',
+                'Accept': 'application/json, text/plain,*/*',
+                'User-Agent': 'Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/78.0.3904.70 Safari/537.36',
+'Sec-Fetch-Site': 'same-origin',
+'Sec-Fetch-Mode': 'cors',
+'x-requested-with': 'XMLHttpRequest',
+                'Accept-Encoding': 'gzip,deflate,br',
+                'Accept-Language': 'zh-CN,zh;q=0.9',
+'Company-Id':'80173240',
+'User-Id':#userId#,
+'Token':#token#,
+'Cookie': #cookies#
+            }</t>
+  </si>
+  <si>
+    <t>{"dptId":"80173243","dptType":3}</t>
+  </si>
+  <si>
+    <t>{
+'pragma': 'no-cache',
+                'Accept': 'application/json, text/plain,*/*',
+                'User-Agent': 'Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/78.0.3904.70 Safari/537.36',
+'Sec-Fetch-Site': 'same-origin',
+'Sec-Fetch-Mode': 'cors',
+'x-requested-with': 'XMLHttpRequest',
+                'Accept-Encoding': 'gzip,deflate,br',
+                'Accept-Language': 'zh-CN,zh;q=0.9',
+'Restful':'{"agreementSignId":29629}',
+'Company-Id':'80173240',
+'User-Id':#userId#,
+'Token':#token#,
+'Cookie': #cookies#
+            }</t>
+  </si>
+  <si>
+    <t>{"pageNo":1,"pageSize":20,"dateTypes":2,"contributorStoreIds":"80173243"}</t>
+  </si>
+  <si>
+    <t>{"pageNo":1,"pageSize":20,"channelType":1,"dateTypes":2,"contributorStoreIds":"80173243"}</t>
+  </si>
+  <si>
+    <t>{"enterpriseId":"57898"}</t>
+  </si>
+  <si>
+    <t>{"projectId":"18219"}</t>
+  </si>
+  <si>
+    <t>{"projectId":"18219","enterpriseId":"57898"}</t>
+  </si>
+  <si>
+    <t>{"enterpriseId":"57898","fundChannelCode":"DY"}</t>
+  </si>
+  <si>
+    <t>{
+'pragma': 'no-cache',
+'Content-Type':'application/json;charset=UTF-8',
+                'Accept': 'application/json, text/plain,*/*',
+                'User-Agent': 'Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/78.0.3904.70 Safari/537.36',
+'Sec-Fetch-Site': 'same-origin',
+'Sec-Fetch-Mode': 'cors',
+'x-requested-with': 'XMLHttpRequest',
+                'Accept-Encoding': 'gzip,deflate,br',
+                'Accept-Language': 'zh-CN,zh;q=0.9',
+'Company-Id':'80173240',
+'User-Id':#userId#,
+'Token':#token#,
+'Cookie': #cookies#
+            }</t>
+  </si>
+  <si>
+    <t>{"branchId":3,"factoringCommissionIds":[#factoringCommissionId#],"bankAccountId":38646,"enterpriseId":"57898"}</t>
+  </si>
+  <si>
+    <t>{
+'pragma': 'no-cache',
+'Content-Type':'application/json;charset=UTF-8',
+                'Accept': 'application/json, text/plain,*/*',
+                'User-Agent': 'Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/78.0.3904.70 Safari/537.36',
+'Sec-Fetch-Site': 'same-origin',
+'Sec-Fetch-Mode': 'cors',
+'x-requested-with': 'XMLHttpRequest',
+                'Accept-Encoding': 'gzip,deflate,br',
+                'Accept-Language': 'zh-CN,zh;q=0.9',
+'Company-Id':'80173240',
+'Restful':#hash_commissionApplyId#,
+'User-Id':#userId#,
+'Token':#token#,
+'Cookie': #cookies#
+            }</t>
   </si>
 </sst>
 </file>
@@ -28587,6 +28947,2216 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:R200"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="10.833333333333334"/>
+    <col min="2" max="2" width="10.833333333333334"/>
+    <col min="3" max="3" width="10.833333333333334"/>
+    <col min="4" max="4" width="10.833333333333334"/>
+    <col min="5" max="5" width="10.833333333333334"/>
+    <col min="6" max="6" width="10.833333333333334"/>
+    <col min="7" max="7" width="10.833333333333334"/>
+    <col min="8" max="8" width="10.833333333333334"/>
+    <col min="9" max="9" width="10.833333333333334"/>
+    <col min="10" max="10" width="10.833333333333334"/>
+    <col min="11" max="11" width="10.833333333333334"/>
+    <col min="12" max="12" width="10.833333333333334"/>
+    <col min="13" max="13" width="10.833333333333334"/>
+    <col min="14" max="14" width="10.833333333333334"/>
+    <col min="15" max="15" width="10.833333333333334"/>
+    <col min="16" max="16" width="10.833333333333334"/>
+    <col min="17" max="17" width="10.833333333333334"/>
+    <col min="18" max="18" width="10.833333333333334"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="36.0">
+      <c r="A1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="93" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="93" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="93" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="93" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="93" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="93" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="93" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="93" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="93" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="93" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="93" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" ht="793.0">
+      <c r="A2" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>363</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="43"/>
+      <c r="G2" s="14" t="s">
+        <v>2132</v>
+      </c>
+      <c r="H2" s="43" t="s">
+        <v>365</v>
+      </c>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43" t="s">
+        <v>2133</v>
+      </c>
+      <c r="K2" s="41" t="s">
+        <v>2134</v>
+      </c>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="43"/>
+    </row>
+    <row r="3" ht="741.0">
+      <c r="A3" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>2135</v>
+      </c>
+      <c r="D3" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="43" t="s">
+        <v>2136</v>
+      </c>
+      <c r="F3" s="43"/>
+      <c r="G3" s="14" t="s">
+        <v>2137</v>
+      </c>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="43"/>
+    </row>
+    <row r="4" ht="767.0">
+      <c r="A4" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>2138</v>
+      </c>
+      <c r="D4" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="43" t="s">
+        <v>2139</v>
+      </c>
+      <c r="F4" s="43"/>
+      <c r="G4" s="14" t="s">
+        <v>2140</v>
+      </c>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43" t="s">
+        <v>879</v>
+      </c>
+      <c r="J4" s="43"/>
+      <c r="K4" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
+    </row>
+    <row r="5" ht="767.0">
+      <c r="A5" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>2141</v>
+      </c>
+      <c r="D5" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="43" t="s">
+        <v>2142</v>
+      </c>
+      <c r="F5" s="43"/>
+      <c r="G5" s="14" t="s">
+        <v>2140</v>
+      </c>
+      <c r="H5" s="43" t="s">
+        <v>2143</v>
+      </c>
+      <c r="I5" s="43" t="s">
+        <v>2144</v>
+      </c>
+      <c r="J5" s="43"/>
+      <c r="K5" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="43"/>
+      <c r="O5" s="43"/>
+      <c r="P5" s="43"/>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="43"/>
+    </row>
+    <row r="6" ht="767.0">
+      <c r="A6" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="B6" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>2145</v>
+      </c>
+      <c r="D6" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="43" t="s">
+        <v>848</v>
+      </c>
+      <c r="F6" s="43"/>
+      <c r="G6" s="14" t="s">
+        <v>2140</v>
+      </c>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43" t="s">
+        <v>2146</v>
+      </c>
+      <c r="J6" s="43"/>
+      <c r="K6" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L6" s="43"/>
+      <c r="M6" s="43"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="43"/>
+      <c r="P6" s="43"/>
+      <c r="Q6" s="43"/>
+      <c r="R6" s="43"/>
+    </row>
+    <row r="7" ht="767.0">
+      <c r="A7" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>2147</v>
+      </c>
+      <c r="D7" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="43" t="s">
+        <v>2148</v>
+      </c>
+      <c r="F7" s="43"/>
+      <c r="G7" s="14" t="s">
+        <v>2140</v>
+      </c>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L7" s="43"/>
+      <c r="M7" s="43"/>
+      <c r="N7" s="43"/>
+      <c r="O7" s="43"/>
+      <c r="P7" s="43"/>
+      <c r="Q7" s="43"/>
+      <c r="R7" s="43"/>
+    </row>
+    <row r="8" ht="819.0">
+      <c r="A8" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="B8" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C8" s="43" t="s">
+        <v>2149</v>
+      </c>
+      <c r="D8" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="43" t="s">
+        <v>2150</v>
+      </c>
+      <c r="F8" s="43"/>
+      <c r="G8" s="14" t="s">
+        <v>2151</v>
+      </c>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
+      <c r="N8" s="43"/>
+      <c r="O8" s="43"/>
+      <c r="P8" s="43"/>
+      <c r="Q8" s="43"/>
+      <c r="R8" s="43"/>
+    </row>
+    <row r="9" ht="767.0">
+      <c r="A9" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="B9" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C9" s="43" t="s">
+        <v>2152</v>
+      </c>
+      <c r="D9" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="43" t="s">
+        <v>863</v>
+      </c>
+      <c r="F9" s="43"/>
+      <c r="G9" s="14" t="s">
+        <v>2140</v>
+      </c>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43" t="s">
+        <v>2153</v>
+      </c>
+      <c r="J9" s="43"/>
+      <c r="K9" s="41" t="s">
+        <v>2154</v>
+      </c>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="43"/>
+      <c r="O9" s="43"/>
+      <c r="P9" s="43"/>
+      <c r="Q9" s="43"/>
+      <c r="R9" s="43"/>
+    </row>
+    <row r="10" ht="767.0">
+      <c r="A10" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C10" s="43" t="s">
+        <v>2155</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="43" t="s">
+        <v>866</v>
+      </c>
+      <c r="F10" s="43"/>
+      <c r="G10" s="14" t="s">
+        <v>2140</v>
+      </c>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43" t="s">
+        <v>2153</v>
+      </c>
+      <c r="J10" s="43"/>
+      <c r="K10" s="41" t="s">
+        <v>2154</v>
+      </c>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="43"/>
+      <c r="R10" s="43"/>
+    </row>
+    <row r="11" ht="767.0">
+      <c r="A11" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="B11" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>2156</v>
+      </c>
+      <c r="D11" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="43" t="s">
+        <v>2157</v>
+      </c>
+      <c r="F11" s="43"/>
+      <c r="G11" s="14" t="s">
+        <v>2140</v>
+      </c>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43" t="s">
+        <v>2158</v>
+      </c>
+      <c r="J11" s="43"/>
+      <c r="K11" s="41" t="s">
+        <v>2154</v>
+      </c>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="43"/>
+      <c r="O11" s="43"/>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="43"/>
+    </row>
+    <row r="12" ht="767.0">
+      <c r="A12" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="B12" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C12" s="43" t="s">
+        <v>2159</v>
+      </c>
+      <c r="D12" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="43" t="s">
+        <v>2160</v>
+      </c>
+      <c r="F12" s="43"/>
+      <c r="G12" s="14" t="s">
+        <v>2140</v>
+      </c>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="43"/>
+      <c r="R12" s="43"/>
+    </row>
+    <row r="13" ht="767.0">
+      <c r="A13" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="B13" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C13" s="43" t="s">
+        <v>2161</v>
+      </c>
+      <c r="D13" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="43" t="s">
+        <v>2162</v>
+      </c>
+      <c r="F13" s="43"/>
+      <c r="G13" s="14" t="s">
+        <v>2140</v>
+      </c>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43" t="s">
+        <v>2163</v>
+      </c>
+      <c r="J13" s="43"/>
+      <c r="K13" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="43"/>
+      <c r="O13" s="43"/>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="43"/>
+      <c r="R13" s="43"/>
+    </row>
+    <row r="14" ht="767.0">
+      <c r="A14" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="B14" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C14" s="43" t="s">
+        <v>2164</v>
+      </c>
+      <c r="D14" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="43" t="s">
+        <v>2165</v>
+      </c>
+      <c r="F14" s="43"/>
+      <c r="G14" s="14" t="s">
+        <v>2140</v>
+      </c>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43" t="s">
+        <v>2163</v>
+      </c>
+      <c r="J14" s="43"/>
+      <c r="K14" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="43"/>
+      <c r="Q14" s="43"/>
+      <c r="R14" s="43"/>
+    </row>
+    <row r="15" ht="767.0">
+      <c r="A15" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="B15" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C15" s="43" t="s">
+        <v>2166</v>
+      </c>
+      <c r="D15" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="43" t="s">
+        <v>2167</v>
+      </c>
+      <c r="F15" s="43"/>
+      <c r="G15" s="14" t="s">
+        <v>2140</v>
+      </c>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43" t="s">
+        <v>2168</v>
+      </c>
+      <c r="J15" s="43"/>
+      <c r="K15" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="43"/>
+      <c r="O15" s="43"/>
+      <c r="P15" s="43"/>
+      <c r="Q15" s="43"/>
+      <c r="R15" s="43"/>
+    </row>
+    <row r="16" ht="767.0">
+      <c r="A16" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="B16" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C16" s="43" t="s">
+        <v>2169</v>
+      </c>
+      <c r="D16" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="43" t="s">
+        <v>2170</v>
+      </c>
+      <c r="F16" s="43"/>
+      <c r="G16" s="14" t="s">
+        <v>2140</v>
+      </c>
+      <c r="H16" s="43" t="s">
+        <v>2171</v>
+      </c>
+      <c r="I16" s="43" t="s">
+        <v>2172</v>
+      </c>
+      <c r="J16" s="43"/>
+      <c r="K16" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L16" s="43"/>
+      <c r="M16" s="43"/>
+      <c r="N16" s="43"/>
+      <c r="O16" s="43"/>
+      <c r="P16" s="43"/>
+      <c r="Q16" s="43"/>
+      <c r="R16" s="43"/>
+    </row>
+    <row r="17" ht="767.0">
+      <c r="A17" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="B17" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C17" s="43" t="s">
+        <v>2173</v>
+      </c>
+      <c r="D17" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="43" t="s">
+        <v>2174</v>
+      </c>
+      <c r="F17" s="43"/>
+      <c r="G17" s="14" t="s">
+        <v>2140</v>
+      </c>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43" t="s">
+        <v>2175</v>
+      </c>
+      <c r="J17" s="43"/>
+      <c r="K17" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L17" s="43"/>
+      <c r="M17" s="43"/>
+      <c r="N17" s="43"/>
+      <c r="O17" s="43"/>
+      <c r="P17" s="43"/>
+      <c r="Q17" s="43"/>
+      <c r="R17" s="43"/>
+    </row>
+    <row r="18" ht="819.0">
+      <c r="A18" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="B18" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C18" s="43" t="s">
+        <v>2176</v>
+      </c>
+      <c r="D18" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="43" t="s">
+        <v>843</v>
+      </c>
+      <c r="F18" s="43"/>
+      <c r="G18" s="14" t="s">
+        <v>2177</v>
+      </c>
+      <c r="H18" s="43" t="s">
+        <v>2178</v>
+      </c>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43" t="s">
+        <v>2179</v>
+      </c>
+      <c r="K18" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L18" s="43"/>
+      <c r="M18" s="43"/>
+      <c r="N18" s="43"/>
+      <c r="O18" s="43"/>
+      <c r="P18" s="43"/>
+      <c r="Q18" s="43"/>
+      <c r="R18" s="43"/>
+    </row>
+    <row r="19" ht="858.0">
+      <c r="A19" s="43" t="s">
+        <v>253</v>
+      </c>
+      <c r="B19" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C19" s="43" t="s">
+        <v>2180</v>
+      </c>
+      <c r="D19" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="43" t="s">
+        <v>851</v>
+      </c>
+      <c r="F19" s="43"/>
+      <c r="G19" s="14" t="s">
+        <v>2181</v>
+      </c>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L19" s="43"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="43"/>
+      <c r="O19" s="43"/>
+      <c r="P19" s="43"/>
+      <c r="Q19" s="43"/>
+      <c r="R19" s="43"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="43"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="43"/>
+      <c r="L20" s="43"/>
+      <c r="M20" s="43"/>
+      <c r="N20" s="43"/>
+      <c r="O20" s="43"/>
+      <c r="P20" s="43"/>
+      <c r="Q20" s="43"/>
+      <c r="R20" s="43"/>
+    </row>
+    <row r="21" ht="611.0">
+      <c r="A21" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="43" t="s">
+        <v>363</v>
+      </c>
+      <c r="D21" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="43"/>
+      <c r="G21" s="12" t="s">
+        <v>2182</v>
+      </c>
+      <c r="H21" s="43" t="s">
+        <v>365</v>
+      </c>
+      <c r="I21" s="43"/>
+      <c r="J21" s="43" t="s">
+        <v>2183</v>
+      </c>
+      <c r="K21" s="39" t="s">
+        <v>2134</v>
+      </c>
+      <c r="L21" s="43"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="43"/>
+      <c r="O21" s="43"/>
+      <c r="P21" s="43"/>
+      <c r="Q21" s="43"/>
+      <c r="R21" s="43"/>
+    </row>
+    <row r="22" ht="650.0">
+      <c r="A22" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="B22" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C22" s="43" t="s">
+        <v>2135</v>
+      </c>
+      <c r="D22" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="43" t="s">
+        <v>2136</v>
+      </c>
+      <c r="F22" s="43"/>
+      <c r="G22" s="14" t="s">
+        <v>2184</v>
+      </c>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L22" s="43"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="43"/>
+      <c r="O22" s="43"/>
+      <c r="P22" s="43"/>
+      <c r="Q22" s="43"/>
+      <c r="R22" s="43"/>
+    </row>
+    <row r="23" ht="676.0">
+      <c r="A23" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C23" s="43" t="s">
+        <v>2138</v>
+      </c>
+      <c r="D23" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="43" t="s">
+        <v>2139</v>
+      </c>
+      <c r="F23" s="43"/>
+      <c r="G23" s="14" t="s">
+        <v>2185</v>
+      </c>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43" t="s">
+        <v>2186</v>
+      </c>
+      <c r="J23" s="43"/>
+      <c r="K23" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L23" s="43"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="43"/>
+      <c r="O23" s="43"/>
+      <c r="P23" s="43"/>
+      <c r="Q23" s="43"/>
+      <c r="R23" s="43"/>
+    </row>
+    <row r="24" ht="676.0">
+      <c r="A24" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="B24" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C24" s="43" t="s">
+        <v>2141</v>
+      </c>
+      <c r="D24" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="43" t="s">
+        <v>2142</v>
+      </c>
+      <c r="F24" s="43"/>
+      <c r="G24" s="14" t="s">
+        <v>2185</v>
+      </c>
+      <c r="H24" s="43" t="s">
+        <v>2143</v>
+      </c>
+      <c r="I24" s="43" t="s">
+        <v>2144</v>
+      </c>
+      <c r="J24" s="43"/>
+      <c r="K24" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L24" s="43"/>
+      <c r="M24" s="43"/>
+      <c r="N24" s="43"/>
+      <c r="O24" s="43"/>
+      <c r="P24" s="43"/>
+      <c r="Q24" s="43"/>
+      <c r="R24" s="43"/>
+    </row>
+    <row r="25" ht="676.0">
+      <c r="A25" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="B25" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C25" s="43" t="s">
+        <v>2145</v>
+      </c>
+      <c r="D25" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="43" t="s">
+        <v>848</v>
+      </c>
+      <c r="F25" s="43"/>
+      <c r="G25" s="14" t="s">
+        <v>2185</v>
+      </c>
+      <c r="H25" s="43"/>
+      <c r="I25" s="43" t="s">
+        <v>2146</v>
+      </c>
+      <c r="J25" s="43"/>
+      <c r="K25" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L25" s="43"/>
+      <c r="M25" s="43"/>
+      <c r="N25" s="43"/>
+      <c r="O25" s="43"/>
+      <c r="P25" s="43"/>
+      <c r="Q25" s="43"/>
+      <c r="R25" s="43"/>
+    </row>
+    <row r="26" ht="676.0">
+      <c r="A26" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="B26" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C26" s="43" t="s">
+        <v>2147</v>
+      </c>
+      <c r="D26" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="43" t="s">
+        <v>2148</v>
+      </c>
+      <c r="F26" s="43"/>
+      <c r="G26" s="14" t="s">
+        <v>2185</v>
+      </c>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L26" s="43"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="43"/>
+      <c r="P26" s="43"/>
+      <c r="Q26" s="43"/>
+      <c r="R26" s="43"/>
+    </row>
+    <row r="27" ht="728.0">
+      <c r="A27" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="B27" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C27" s="43" t="s">
+        <v>2149</v>
+      </c>
+      <c r="D27" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="43" t="s">
+        <v>2150</v>
+      </c>
+      <c r="F27" s="43"/>
+      <c r="G27" s="14" t="s">
+        <v>2187</v>
+      </c>
+      <c r="H27" s="43"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="43"/>
+      <c r="K27" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L27" s="43"/>
+      <c r="M27" s="43"/>
+      <c r="N27" s="43"/>
+      <c r="O27" s="43"/>
+      <c r="P27" s="43"/>
+      <c r="Q27" s="43"/>
+      <c r="R27" s="43"/>
+    </row>
+    <row r="28" ht="676.0">
+      <c r="A28" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="B28" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C28" s="43" t="s">
+        <v>2152</v>
+      </c>
+      <c r="D28" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28" s="43" t="s">
+        <v>863</v>
+      </c>
+      <c r="F28" s="43"/>
+      <c r="G28" s="14" t="s">
+        <v>2185</v>
+      </c>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43" t="s">
+        <v>2188</v>
+      </c>
+      <c r="J28" s="43"/>
+      <c r="K28" s="41" t="s">
+        <v>2154</v>
+      </c>
+      <c r="L28" s="43"/>
+      <c r="M28" s="43"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="43"/>
+      <c r="P28" s="43"/>
+      <c r="Q28" s="43"/>
+      <c r="R28" s="43"/>
+    </row>
+    <row r="29" ht="676.0">
+      <c r="A29" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="B29" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C29" s="43" t="s">
+        <v>2155</v>
+      </c>
+      <c r="D29" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" s="43" t="s">
+        <v>866</v>
+      </c>
+      <c r="F29" s="43"/>
+      <c r="G29" s="14" t="s">
+        <v>2185</v>
+      </c>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43" t="s">
+        <v>2188</v>
+      </c>
+      <c r="J29" s="43"/>
+      <c r="K29" s="41" t="s">
+        <v>2154</v>
+      </c>
+      <c r="L29" s="43"/>
+      <c r="M29" s="43"/>
+      <c r="N29" s="43"/>
+      <c r="O29" s="43"/>
+      <c r="P29" s="43"/>
+      <c r="Q29" s="43"/>
+      <c r="R29" s="43"/>
+    </row>
+    <row r="30" ht="676.0">
+      <c r="A30" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="B30" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C30" s="43" t="s">
+        <v>2156</v>
+      </c>
+      <c r="D30" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="43" t="s">
+        <v>2157</v>
+      </c>
+      <c r="F30" s="43"/>
+      <c r="G30" s="14" t="s">
+        <v>2185</v>
+      </c>
+      <c r="H30" s="43"/>
+      <c r="I30" s="43" t="s">
+        <v>2189</v>
+      </c>
+      <c r="J30" s="43"/>
+      <c r="K30" s="41" t="s">
+        <v>2154</v>
+      </c>
+      <c r="L30" s="43"/>
+      <c r="M30" s="43"/>
+      <c r="N30" s="43"/>
+      <c r="O30" s="43"/>
+      <c r="P30" s="43"/>
+      <c r="Q30" s="43"/>
+      <c r="R30" s="43"/>
+    </row>
+    <row r="31" ht="676.0">
+      <c r="A31" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="B31" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C31" s="43" t="s">
+        <v>2159</v>
+      </c>
+      <c r="D31" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" s="43" t="s">
+        <v>2160</v>
+      </c>
+      <c r="F31" s="43"/>
+      <c r="G31" s="14" t="s">
+        <v>2185</v>
+      </c>
+      <c r="H31" s="43"/>
+      <c r="I31" s="43"/>
+      <c r="J31" s="43"/>
+      <c r="K31" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L31" s="43"/>
+      <c r="M31" s="43"/>
+      <c r="N31" s="43"/>
+      <c r="O31" s="43"/>
+      <c r="P31" s="43"/>
+      <c r="Q31" s="43"/>
+      <c r="R31" s="43"/>
+    </row>
+    <row r="32" ht="676.0">
+      <c r="A32" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="B32" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C32" s="43" t="s">
+        <v>2161</v>
+      </c>
+      <c r="D32" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" s="43" t="s">
+        <v>2162</v>
+      </c>
+      <c r="F32" s="43"/>
+      <c r="G32" s="14" t="s">
+        <v>2185</v>
+      </c>
+      <c r="H32" s="43"/>
+      <c r="I32" s="43" t="s">
+        <v>2190</v>
+      </c>
+      <c r="J32" s="43"/>
+      <c r="K32" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L32" s="43"/>
+      <c r="M32" s="43"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="43"/>
+      <c r="P32" s="43"/>
+      <c r="Q32" s="43"/>
+      <c r="R32" s="43"/>
+    </row>
+    <row r="33" ht="676.0">
+      <c r="A33" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="B33" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C33" s="43" t="s">
+        <v>2164</v>
+      </c>
+      <c r="D33" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" s="43" t="s">
+        <v>2165</v>
+      </c>
+      <c r="F33" s="43"/>
+      <c r="G33" s="14" t="s">
+        <v>2185</v>
+      </c>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43" t="s">
+        <v>2190</v>
+      </c>
+      <c r="J33" s="43"/>
+      <c r="K33" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L33" s="43"/>
+      <c r="M33" s="43"/>
+      <c r="N33" s="43"/>
+      <c r="O33" s="43"/>
+      <c r="P33" s="43"/>
+      <c r="Q33" s="43"/>
+      <c r="R33" s="43"/>
+    </row>
+    <row r="34" ht="676.0">
+      <c r="A34" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C34" s="43" t="s">
+        <v>2166</v>
+      </c>
+      <c r="D34" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" s="43" t="s">
+        <v>2167</v>
+      </c>
+      <c r="F34" s="43"/>
+      <c r="G34" s="14" t="s">
+        <v>2185</v>
+      </c>
+      <c r="H34" s="43"/>
+      <c r="I34" s="43" t="s">
+        <v>2191</v>
+      </c>
+      <c r="J34" s="43"/>
+      <c r="K34" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L34" s="43"/>
+      <c r="M34" s="43"/>
+      <c r="N34" s="43"/>
+      <c r="O34" s="43"/>
+      <c r="P34" s="43"/>
+      <c r="Q34" s="43"/>
+      <c r="R34" s="43"/>
+    </row>
+    <row r="35" ht="676.0">
+      <c r="A35" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C35" s="43" t="s">
+        <v>2169</v>
+      </c>
+      <c r="D35" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35" s="43" t="s">
+        <v>2170</v>
+      </c>
+      <c r="F35" s="43"/>
+      <c r="G35" s="14" t="s">
+        <v>2185</v>
+      </c>
+      <c r="H35" s="43" t="s">
+        <v>2171</v>
+      </c>
+      <c r="I35" s="43" t="s">
+        <v>2192</v>
+      </c>
+      <c r="J35" s="43"/>
+      <c r="K35" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L35" s="43"/>
+      <c r="M35" s="43"/>
+      <c r="N35" s="43"/>
+      <c r="O35" s="43"/>
+      <c r="P35" s="43"/>
+      <c r="Q35" s="43"/>
+      <c r="R35" s="43"/>
+    </row>
+    <row r="36" ht="676.0">
+      <c r="A36" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="B36" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C36" s="43" t="s">
+        <v>2173</v>
+      </c>
+      <c r="D36" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E36" s="43" t="s">
+        <v>2174</v>
+      </c>
+      <c r="F36" s="43"/>
+      <c r="G36" s="14" t="s">
+        <v>2185</v>
+      </c>
+      <c r="H36" s="43"/>
+      <c r="I36" s="43" t="s">
+        <v>2193</v>
+      </c>
+      <c r="J36" s="43"/>
+      <c r="K36" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L36" s="43"/>
+      <c r="M36" s="43"/>
+      <c r="N36" s="43"/>
+      <c r="O36" s="43"/>
+      <c r="P36" s="43"/>
+      <c r="Q36" s="43"/>
+      <c r="R36" s="43"/>
+    </row>
+    <row r="37" ht="728.0">
+      <c r="A37" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="B37" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C37" s="43" t="s">
+        <v>2176</v>
+      </c>
+      <c r="D37" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="43" t="s">
+        <v>843</v>
+      </c>
+      <c r="F37" s="43"/>
+      <c r="G37" s="14" t="s">
+        <v>2194</v>
+      </c>
+      <c r="H37" s="43" t="s">
+        <v>2178</v>
+      </c>
+      <c r="I37" s="43"/>
+      <c r="J37" s="43" t="s">
+        <v>2195</v>
+      </c>
+      <c r="K37" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L37" s="43"/>
+      <c r="M37" s="43"/>
+      <c r="N37" s="43"/>
+      <c r="O37" s="43"/>
+      <c r="P37" s="43"/>
+      <c r="Q37" s="43"/>
+      <c r="R37" s="43"/>
+    </row>
+    <row r="38" ht="767.0">
+      <c r="A38" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="B38" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C38" s="43" t="s">
+        <v>2180</v>
+      </c>
+      <c r="D38" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" s="43" t="s">
+        <v>851</v>
+      </c>
+      <c r="F38" s="43"/>
+      <c r="G38" s="14" t="s">
+        <v>2196</v>
+      </c>
+      <c r="H38" s="43"/>
+      <c r="I38" s="43"/>
+      <c r="J38" s="43"/>
+      <c r="K38" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L38" s="43"/>
+      <c r="M38" s="43"/>
+      <c r="N38" s="43"/>
+      <c r="O38" s="43"/>
+      <c r="P38" s="43"/>
+      <c r="Q38" s="43"/>
+      <c r="R38" s="43"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="43"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="43"/>
+      <c r="D39" s="43"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="43"/>
+      <c r="H39" s="43"/>
+      <c r="I39" s="43"/>
+      <c r="J39" s="43"/>
+      <c r="K39" s="43"/>
+      <c r="L39" s="43"/>
+      <c r="M39" s="43"/>
+      <c r="N39" s="43"/>
+      <c r="O39" s="43"/>
+      <c r="P39" s="43"/>
+      <c r="Q39" s="43"/>
+      <c r="R39" s="43"/>
+    </row>
+    <row r="40" ht="611.0">
+      <c r="A40" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="43" t="s">
+        <v>363</v>
+      </c>
+      <c r="D40" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="F40" s="43"/>
+      <c r="G40" s="12" t="s">
+        <v>2182</v>
+      </c>
+      <c r="H40" s="43" t="s">
+        <v>365</v>
+      </c>
+      <c r="I40" s="43"/>
+      <c r="J40" s="43" t="s">
+        <v>2183</v>
+      </c>
+      <c r="K40" s="39" t="s">
+        <v>2134</v>
+      </c>
+      <c r="L40" s="43"/>
+      <c r="M40" s="43"/>
+      <c r="N40" s="43"/>
+      <c r="O40" s="43"/>
+      <c r="P40" s="43"/>
+      <c r="Q40" s="43"/>
+      <c r="R40" s="43"/>
+    </row>
+    <row r="41" ht="650.0">
+      <c r="A41" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C41" s="43" t="s">
+        <v>2135</v>
+      </c>
+      <c r="D41" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E41" s="43" t="s">
+        <v>2136</v>
+      </c>
+      <c r="F41" s="43"/>
+      <c r="G41" s="14" t="s">
+        <v>2184</v>
+      </c>
+      <c r="H41" s="43"/>
+      <c r="I41" s="43"/>
+      <c r="J41" s="43"/>
+      <c r="K41" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L41" s="43"/>
+      <c r="M41" s="43"/>
+      <c r="N41" s="43"/>
+      <c r="O41" s="43"/>
+      <c r="P41" s="43"/>
+      <c r="Q41" s="43"/>
+      <c r="R41" s="43"/>
+    </row>
+    <row r="42" ht="676.0">
+      <c r="A42" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C42" s="43" t="s">
+        <v>2138</v>
+      </c>
+      <c r="D42" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E42" s="43" t="s">
+        <v>2139</v>
+      </c>
+      <c r="F42" s="43"/>
+      <c r="G42" s="14" t="s">
+        <v>2185</v>
+      </c>
+      <c r="H42" s="43"/>
+      <c r="I42" s="43" t="s">
+        <v>2186</v>
+      </c>
+      <c r="J42" s="43"/>
+      <c r="K42" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L42" s="43"/>
+      <c r="M42" s="43"/>
+      <c r="N42" s="43"/>
+      <c r="O42" s="43"/>
+      <c r="P42" s="43"/>
+      <c r="Q42" s="43"/>
+      <c r="R42" s="43"/>
+    </row>
+    <row r="43" ht="676.0">
+      <c r="A43" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C43" s="43" t="s">
+        <v>2141</v>
+      </c>
+      <c r="D43" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E43" s="43" t="s">
+        <v>2142</v>
+      </c>
+      <c r="F43" s="43"/>
+      <c r="G43" s="14" t="s">
+        <v>2185</v>
+      </c>
+      <c r="H43" s="43" t="s">
+        <v>2143</v>
+      </c>
+      <c r="I43" s="43" t="s">
+        <v>2144</v>
+      </c>
+      <c r="J43" s="43"/>
+      <c r="K43" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L43" s="43"/>
+      <c r="M43" s="43"/>
+      <c r="N43" s="43"/>
+      <c r="O43" s="43"/>
+      <c r="P43" s="43"/>
+      <c r="Q43" s="43"/>
+      <c r="R43" s="43"/>
+    </row>
+    <row r="44" ht="676.0">
+      <c r="A44" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C44" s="43" t="s">
+        <v>2145</v>
+      </c>
+      <c r="D44" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" s="43" t="s">
+        <v>848</v>
+      </c>
+      <c r="F44" s="43"/>
+      <c r="G44" s="14" t="s">
+        <v>2185</v>
+      </c>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43" t="s">
+        <v>2146</v>
+      </c>
+      <c r="J44" s="43"/>
+      <c r="K44" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L44" s="43"/>
+      <c r="M44" s="43"/>
+      <c r="N44" s="43"/>
+      <c r="O44" s="43"/>
+      <c r="P44" s="43"/>
+      <c r="Q44" s="43"/>
+      <c r="R44" s="43"/>
+    </row>
+    <row r="45" ht="676.0">
+      <c r="A45" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C45" s="43" t="s">
+        <v>2147</v>
+      </c>
+      <c r="D45" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E45" s="43" t="s">
+        <v>2148</v>
+      </c>
+      <c r="F45" s="43"/>
+      <c r="G45" s="14" t="s">
+        <v>2185</v>
+      </c>
+      <c r="H45" s="43"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
+      <c r="K45" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L45" s="43"/>
+      <c r="M45" s="43"/>
+      <c r="N45" s="43"/>
+      <c r="O45" s="43"/>
+      <c r="P45" s="43"/>
+      <c r="Q45" s="43"/>
+      <c r="R45" s="43"/>
+    </row>
+    <row r="46" ht="728.0">
+      <c r="A46" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C46" s="43" t="s">
+        <v>2149</v>
+      </c>
+      <c r="D46" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E46" s="43" t="s">
+        <v>2150</v>
+      </c>
+      <c r="F46" s="43"/>
+      <c r="G46" s="14" t="s">
+        <v>2187</v>
+      </c>
+      <c r="H46" s="43"/>
+      <c r="I46" s="43"/>
+      <c r="J46" s="43"/>
+      <c r="K46" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L46" s="43"/>
+      <c r="M46" s="43"/>
+      <c r="N46" s="43"/>
+      <c r="O46" s="43"/>
+      <c r="P46" s="43"/>
+      <c r="Q46" s="43"/>
+      <c r="R46" s="43"/>
+    </row>
+    <row r="47" ht="676.0">
+      <c r="A47" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C47" s="43" t="s">
+        <v>2152</v>
+      </c>
+      <c r="D47" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E47" s="43" t="s">
+        <v>863</v>
+      </c>
+      <c r="F47" s="43"/>
+      <c r="G47" s="14" t="s">
+        <v>2185</v>
+      </c>
+      <c r="H47" s="43"/>
+      <c r="I47" s="43" t="s">
+        <v>2188</v>
+      </c>
+      <c r="J47" s="43"/>
+      <c r="K47" s="41" t="s">
+        <v>2154</v>
+      </c>
+      <c r="L47" s="43"/>
+      <c r="M47" s="43"/>
+      <c r="N47" s="43"/>
+      <c r="O47" s="43"/>
+      <c r="P47" s="43"/>
+      <c r="Q47" s="43"/>
+      <c r="R47" s="43"/>
+    </row>
+    <row r="48" ht="676.0">
+      <c r="A48" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C48" s="43" t="s">
+        <v>2155</v>
+      </c>
+      <c r="D48" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E48" s="43" t="s">
+        <v>866</v>
+      </c>
+      <c r="F48" s="43"/>
+      <c r="G48" s="14" t="s">
+        <v>2185</v>
+      </c>
+      <c r="H48" s="43"/>
+      <c r="I48" s="43" t="s">
+        <v>2188</v>
+      </c>
+      <c r="J48" s="43"/>
+      <c r="K48" s="41" t="s">
+        <v>2154</v>
+      </c>
+      <c r="L48" s="43"/>
+      <c r="M48" s="43"/>
+      <c r="N48" s="43"/>
+      <c r="O48" s="43"/>
+      <c r="P48" s="43"/>
+      <c r="Q48" s="43"/>
+      <c r="R48" s="43"/>
+    </row>
+    <row r="49" ht="676.0">
+      <c r="A49" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C49" s="43" t="s">
+        <v>2156</v>
+      </c>
+      <c r="D49" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E49" s="43" t="s">
+        <v>2157</v>
+      </c>
+      <c r="F49" s="43"/>
+      <c r="G49" s="14" t="s">
+        <v>2185</v>
+      </c>
+      <c r="H49" s="43"/>
+      <c r="I49" s="43" t="s">
+        <v>2189</v>
+      </c>
+      <c r="J49" s="43"/>
+      <c r="K49" s="41" t="s">
+        <v>2154</v>
+      </c>
+      <c r="L49" s="43"/>
+      <c r="M49" s="43"/>
+      <c r="N49" s="43"/>
+      <c r="O49" s="43"/>
+      <c r="P49" s="43"/>
+      <c r="Q49" s="43"/>
+      <c r="R49" s="43"/>
+    </row>
+    <row r="50" ht="676.0">
+      <c r="A50" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B50" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C50" s="43" t="s">
+        <v>2159</v>
+      </c>
+      <c r="D50" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E50" s="43" t="s">
+        <v>2160</v>
+      </c>
+      <c r="F50" s="43"/>
+      <c r="G50" s="14" t="s">
+        <v>2185</v>
+      </c>
+      <c r="H50" s="43"/>
+      <c r="I50" s="43"/>
+      <c r="J50" s="43"/>
+      <c r="K50" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L50" s="43"/>
+      <c r="M50" s="43"/>
+      <c r="N50" s="43"/>
+      <c r="O50" s="43"/>
+      <c r="P50" s="43"/>
+      <c r="Q50" s="43"/>
+      <c r="R50" s="43"/>
+    </row>
+    <row r="51" ht="676.0">
+      <c r="A51" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B51" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C51" s="43" t="s">
+        <v>2161</v>
+      </c>
+      <c r="D51" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E51" s="43" t="s">
+        <v>2162</v>
+      </c>
+      <c r="F51" s="43"/>
+      <c r="G51" s="14" t="s">
+        <v>2185</v>
+      </c>
+      <c r="H51" s="43"/>
+      <c r="I51" s="43" t="s">
+        <v>2190</v>
+      </c>
+      <c r="J51" s="43"/>
+      <c r="K51" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L51" s="43"/>
+      <c r="M51" s="43"/>
+      <c r="N51" s="43"/>
+      <c r="O51" s="43"/>
+      <c r="P51" s="43"/>
+      <c r="Q51" s="43"/>
+      <c r="R51" s="43"/>
+    </row>
+    <row r="52" ht="676.0">
+      <c r="A52" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C52" s="43" t="s">
+        <v>2164</v>
+      </c>
+      <c r="D52" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E52" s="43" t="s">
+        <v>2165</v>
+      </c>
+      <c r="F52" s="43"/>
+      <c r="G52" s="14" t="s">
+        <v>2185</v>
+      </c>
+      <c r="H52" s="43"/>
+      <c r="I52" s="43" t="s">
+        <v>2190</v>
+      </c>
+      <c r="J52" s="43"/>
+      <c r="K52" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L52" s="43"/>
+      <c r="M52" s="43"/>
+      <c r="N52" s="43"/>
+      <c r="O52" s="43"/>
+      <c r="P52" s="43"/>
+      <c r="Q52" s="43"/>
+      <c r="R52" s="43"/>
+    </row>
+    <row r="53" ht="676.0">
+      <c r="A53" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C53" s="43" t="s">
+        <v>2166</v>
+      </c>
+      <c r="D53" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E53" s="43" t="s">
+        <v>2167</v>
+      </c>
+      <c r="F53" s="43"/>
+      <c r="G53" s="14" t="s">
+        <v>2185</v>
+      </c>
+      <c r="H53" s="43"/>
+      <c r="I53" s="43" t="s">
+        <v>2191</v>
+      </c>
+      <c r="J53" s="43"/>
+      <c r="K53" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L53" s="43"/>
+      <c r="M53" s="43"/>
+      <c r="N53" s="43"/>
+      <c r="O53" s="43"/>
+      <c r="P53" s="43"/>
+      <c r="Q53" s="43"/>
+      <c r="R53" s="43"/>
+    </row>
+    <row r="54" ht="676.0">
+      <c r="A54" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C54" s="43" t="s">
+        <v>2169</v>
+      </c>
+      <c r="D54" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E54" s="43" t="s">
+        <v>2170</v>
+      </c>
+      <c r="F54" s="43"/>
+      <c r="G54" s="14" t="s">
+        <v>2185</v>
+      </c>
+      <c r="H54" s="43" t="s">
+        <v>2171</v>
+      </c>
+      <c r="I54" s="43" t="s">
+        <v>2192</v>
+      </c>
+      <c r="J54" s="43"/>
+      <c r="K54" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L54" s="43"/>
+      <c r="M54" s="43"/>
+      <c r="N54" s="43"/>
+      <c r="O54" s="43"/>
+      <c r="P54" s="43"/>
+      <c r="Q54" s="43"/>
+      <c r="R54" s="43"/>
+    </row>
+    <row r="55" ht="676.0">
+      <c r="A55" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C55" s="43" t="s">
+        <v>2173</v>
+      </c>
+      <c r="D55" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E55" s="43" t="s">
+        <v>2174</v>
+      </c>
+      <c r="F55" s="43"/>
+      <c r="G55" s="14" t="s">
+        <v>2185</v>
+      </c>
+      <c r="H55" s="43"/>
+      <c r="I55" s="43" t="s">
+        <v>2193</v>
+      </c>
+      <c r="J55" s="43"/>
+      <c r="K55" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L55" s="43"/>
+      <c r="M55" s="43"/>
+      <c r="N55" s="43"/>
+      <c r="O55" s="43"/>
+      <c r="P55" s="43"/>
+      <c r="Q55" s="43"/>
+      <c r="R55" s="43"/>
+    </row>
+    <row r="56" ht="728.0">
+      <c r="A56" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C56" s="43" t="s">
+        <v>2176</v>
+      </c>
+      <c r="D56" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="E56" s="43" t="s">
+        <v>843</v>
+      </c>
+      <c r="F56" s="43"/>
+      <c r="G56" s="14" t="s">
+        <v>2194</v>
+      </c>
+      <c r="H56" s="43" t="s">
+        <v>2178</v>
+      </c>
+      <c r="I56" s="43"/>
+      <c r="J56" s="43" t="s">
+        <v>2195</v>
+      </c>
+      <c r="K56" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L56" s="43"/>
+      <c r="M56" s="43"/>
+      <c r="N56" s="43"/>
+      <c r="O56" s="43"/>
+      <c r="P56" s="43"/>
+      <c r="Q56" s="43"/>
+      <c r="R56" s="43"/>
+    </row>
+    <row r="57" ht="767.0">
+      <c r="A57" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57" s="43" t="s">
+        <v>803</v>
+      </c>
+      <c r="C57" s="43" t="s">
+        <v>2180</v>
+      </c>
+      <c r="D57" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57" s="43" t="s">
+        <v>851</v>
+      </c>
+      <c r="F57" s="43"/>
+      <c r="G57" s="14" t="s">
+        <v>2196</v>
+      </c>
+      <c r="H57" s="43"/>
+      <c r="I57" s="43"/>
+      <c r="J57" s="43"/>
+      <c r="K57" s="41" t="s">
+        <v>875</v>
+      </c>
+      <c r="L57" s="43"/>
+      <c r="M57" s="43"/>
+      <c r="N57" s="43"/>
+      <c r="O57" s="43"/>
+      <c r="P57" s="43"/>
+      <c r="Q57" s="43"/>
+      <c r="R57" s="43"/>
+    </row>
+    <row r="58"/>
+    <row r="59"/>
+    <row r="60"/>
+    <row r="61"/>
+    <row r="62"/>
+    <row r="63"/>
+    <row r="64"/>
+    <row r="65"/>
+    <row r="66"/>
+    <row r="67"/>
+    <row r="68"/>
+    <row r="69"/>
+    <row r="70"/>
+    <row r="71"/>
+    <row r="72"/>
+    <row r="73"/>
+    <row r="74"/>
+    <row r="75"/>
+    <row r="76"/>
+    <row r="77"/>
+    <row r="78"/>
+    <row r="79"/>
+    <row r="80"/>
+    <row r="81"/>
+    <row r="82"/>
+    <row r="83"/>
+    <row r="84"/>
+    <row r="85"/>
+    <row r="86"/>
+    <row r="87"/>
+    <row r="88"/>
+    <row r="89"/>
+    <row r="90"/>
+    <row r="91"/>
+    <row r="92"/>
+    <row r="93"/>
+    <row r="94"/>
+    <row r="95"/>
+    <row r="96"/>
+    <row r="97"/>
+    <row r="98"/>
+    <row r="99"/>
+    <row r="100"/>
+    <row r="101"/>
+    <row r="102"/>
+    <row r="103"/>
+    <row r="104"/>
+    <row r="105"/>
+    <row r="106"/>
+    <row r="107"/>
+    <row r="108"/>
+    <row r="109"/>
+    <row r="110"/>
+    <row r="111"/>
+    <row r="112"/>
+    <row r="113"/>
+    <row r="114"/>
+    <row r="115"/>
+    <row r="116"/>
+    <row r="117"/>
+    <row r="118"/>
+    <row r="119"/>
+    <row r="120"/>
+    <row r="121"/>
+    <row r="122"/>
+    <row r="123"/>
+    <row r="124"/>
+    <row r="125"/>
+    <row r="126"/>
+    <row r="127"/>
+    <row r="128"/>
+    <row r="129"/>
+    <row r="130"/>
+    <row r="131"/>
+    <row r="132"/>
+    <row r="133"/>
+    <row r="134"/>
+    <row r="135"/>
+    <row r="136"/>
+    <row r="137"/>
+    <row r="138"/>
+    <row r="139"/>
+    <row r="140"/>
+    <row r="141"/>
+    <row r="142"/>
+    <row r="143"/>
+    <row r="144"/>
+    <row r="145"/>
+    <row r="146"/>
+    <row r="147"/>
+    <row r="148"/>
+    <row r="149"/>
+    <row r="150"/>
+    <row r="151"/>
+    <row r="152"/>
+    <row r="153"/>
+    <row r="154"/>
+    <row r="155"/>
+    <row r="156"/>
+    <row r="157"/>
+    <row r="158"/>
+    <row r="159"/>
+    <row r="160"/>
+    <row r="161"/>
+    <row r="162"/>
+    <row r="163"/>
+    <row r="164"/>
+    <row r="165"/>
+    <row r="166"/>
+    <row r="167"/>
+    <row r="168"/>
+    <row r="169"/>
+    <row r="170"/>
+    <row r="171"/>
+    <row r="172"/>
+    <row r="173"/>
+    <row r="174"/>
+    <row r="175"/>
+    <row r="176"/>
+    <row r="177"/>
+    <row r="178"/>
+    <row r="179"/>
+    <row r="180"/>
+    <row r="181"/>
+    <row r="182"/>
+    <row r="183"/>
+    <row r="184"/>
+    <row r="185"/>
+    <row r="186"/>
+    <row r="187"/>
+    <row r="188"/>
+    <row r="189"/>
+    <row r="190"/>
+    <row r="191"/>
+    <row r="192"/>
+    <row r="193"/>
+    <row r="194"/>
+    <row r="195"/>
+    <row r="196"/>
+    <row r="197"/>
+    <row r="198"/>
+    <row r="199"/>
+    <row r="200"/>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:R199"/>

</xml_diff>